<commit_message>
Updated timesheet - Vinoth
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet .xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50AB7F8B-2D25-416A-B259-4AF60DAEFCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E8D1F9C-F849-4EB1-BCE8-38EBB1AE71EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="Day11 ( 19-04-2022 )" sheetId="51" r:id="rId9"/>
     <sheet name="Day12 ( 20-04-2022 )" sheetId="52" r:id="rId10"/>
     <sheet name="Day13 ( 21-04-2022 )" sheetId="53" r:id="rId11"/>
+    <sheet name="Day14 ( 22-04-2022 )" sheetId="54" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="196">
   <si>
     <t>Column1</t>
   </si>
@@ -783,7 +784,10 @@
     <t>8.45 am - 9.00 am : Brainstorming with Team
 9.00 am - 10.30 am : Added operations(available responses, Employee) 
 10.45 am - 11.30 am : Refined operations (Project, Departement,cancellation reason)
-11.30 am - 12.30 am : Refined operations in Drive model and aligned Logical Diagram</t>
+11.30 am - 12.30 am : Refined operations in Drive model and aligned Logical Diagram1.30 - 2.30 : Refined Operations
+2.30 - 3.30 : Discussed nfr and system architecture
+2.50 - 4.00 : Review with Rafi (Data model operations, NFR)
+4.30 - 5.00 : Discussed MOM</t>
   </si>
   <si>
     <t xml:space="preserve">Seeking for more NFR and Pain points, Interactions. </t>
@@ -795,6 +799,11 @@
 11.15 am - 11:30 : Break and clarification (Total number of NFR)
 11:30 am - 12.00 pm : shallow (sample) and deep (final)
 12.00 pm - 12.15 pm : Clarity about NFR, Refinement of flow.  </t>
+  </si>
+  <si>
+    <t>8.45 - 9.00 : Brainstorming with Team
+9.00 - 10.40 : Updated data model (Drive)
+11.00 - 12.30 : refined data model (Pool, Pool member, Location, Department, Project)</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1211,539 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="231">
+  <dxfs count="252">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -7069,319 +7610,348 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="230" dataDxfId="229" headerRowBorderDxfId="227" tableBorderDxfId="228" totalsRowBorderDxfId="226">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="251" dataDxfId="250" headerRowBorderDxfId="248" tableBorderDxfId="249" totalsRowBorderDxfId="247">
   <autoFilter ref="B9:H19" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="225"/>
-    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="224"/>
-    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="223"/>
-    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="222"/>
-    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="221"/>
-    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="220"/>
-    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="219"/>
+    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="246"/>
+    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="245"/>
+    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="244"/>
+    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="243"/>
+    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="242"/>
+    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="241"/>
+    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="240"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{567599D8-F2AC-4863-A31E-867E4662A188}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{567599D8-F2AC-4863-A31E-867E4662A188}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6862ACD5-06E8-4C76-86B8-0FBF46C719AB}" name="Resource Name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{2FEAF882-A5EF-4611-91BB-CAEDE2BD0142}" name="In-progress" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{FB3D921D-555F-47F7-9140-AB8143CB71BA}" name="Done" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{BD8867CA-8566-48C2-BDB8-839066AC235A}" name="Discarded / Hold" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{F71E5005-E794-436C-8ABB-93D21EB0BD11}" name="Hours Spent - Project" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{53117683-12E5-4475-8EE2-ECA8DBFEEF45}" name="Hours Spent - Non Project" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{A1C72867-09F6-497F-ACF5-1458D252B64F}" name="Comments" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{6862ACD5-06E8-4C76-86B8-0FBF46C719AB}" name="Resource Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{2FEAF882-A5EF-4611-91BB-CAEDE2BD0142}" name="In-progress" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{FB3D921D-555F-47F7-9140-AB8143CB71BA}" name="Done" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{BD8867CA-8566-48C2-BDB8-839066AC235A}" name="Discarded / Hold" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{F71E5005-E794-436C-8ABB-93D21EB0BD11}" name="Hours Spent - Project" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{53117683-12E5-4475-8EE2-ECA8DBFEEF45}" name="Hours Spent - Non Project" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{A1C72867-09F6-497F-ACF5-1458D252B64F}" name="Comments" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217" headerRowBorderDxfId="215" tableBorderDxfId="216" totalsRowBorderDxfId="214">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="239" dataDxfId="238" headerRowBorderDxfId="236" tableBorderDxfId="237" totalsRowBorderDxfId="235">
   <autoFilter ref="B4:E6" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="213"/>
-    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="212"/>
-    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="211"/>
-    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="210"/>
+    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="234"/>
+    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="233"/>
+    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="232"/>
+    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="231"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3AB7E480-AA41-45EE-8BD2-799B66CF977F}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3AB7E480-AA41-45EE-8BD2-799B66CF977F}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5F5286EA-BF04-4F20-B734-0734EC625276}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{2666153F-F4E8-45C3-9985-38E5471A82F0}" name="Column2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{ED99E108-F673-4294-9E8D-A329582DF55B}" name="Column3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{B0F02456-D0DE-4E93-9016-90FA89E16184}" name="Column4" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{5F5286EA-BF04-4F20-B734-0734EC625276}" name="Column1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{2666153F-F4E8-45C3-9985-38E5471A82F0}" name="Column2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{ED99E108-F673-4294-9E8D-A329582DF55B}" name="Column3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{B0F02456-D0DE-4E93-9016-90FA89E16184}" name="Column4" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}" name="Table2621016182022" displayName="Table2621016182022" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}" name="Table2621016182022" displayName="Table2621016182022" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
   <autoFilter ref="B7:H17" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F31F1358-1BCD-4E28-8DE6-55060AD83C78}" name="Resource Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{85795525-35CB-4867-B9E8-8424F3C504C7}" name="In-progress" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{14491860-1E0F-4FC2-B40C-7BFA09F08AD3}" name="Done" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{4121DE0A-E31D-4416-93C4-5D79C06CB436}" name="Discarded / Hold" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{42DAEAF5-4695-460C-A7C8-11CA5A06441F}" name="Hours Spent - Project" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{5A90E8D4-8EBC-413F-9D20-BC476DDDDA89}" name="Hours Spent - Non Project" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{CDA42C61-7D2B-4220-801B-18B140C01D85}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{F31F1358-1BCD-4E28-8DE6-55060AD83C78}" name="Resource Name" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{85795525-35CB-4867-B9E8-8424F3C504C7}" name="In-progress" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{14491860-1E0F-4FC2-B40C-7BFA09F08AD3}" name="Done" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{4121DE0A-E31D-4416-93C4-5D79C06CB436}" name="Discarded / Hold" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{42DAEAF5-4695-460C-A7C8-11CA5A06441F}" name="Hours Spent - Project" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{5A90E8D4-8EBC-413F-9D20-BC476DDDDA89}" name="Hours Spent - Non Project" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{CDA42C61-7D2B-4220-801B-18B140C01D85}" name="Comments" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}" name="Table3751117192123" displayName="Table3751117192123" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}" name="Table3751117192123" displayName="Table3751117192123" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
   <autoFilter ref="B2:E4" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A361ACD1-4939-41DE-8AA2-8A2C23550B5A}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{ADE6E992-B56C-47A2-8484-0F95117DFA87}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5D6FC945-76E2-4A8F-A729-023221CFF273}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{F5B29A6E-68F5-487F-AE11-943B1309598F}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A361ACD1-4939-41DE-8AA2-8A2C23550B5A}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{ADE6E992-B56C-47A2-8484-0F95117DFA87}" name="Column2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{5D6FC945-76E2-4A8F-A729-023221CFF273}" name="Column3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{F5B29A6E-68F5-487F-AE11-943B1309598F}" name="Column4" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{8F6F8532-A566-4B0B-AECF-B2BE04EC37C4}" name="Table262101618202224" displayName="Table262101618202224" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B7:H17" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C59EFFEB-6F71-4923-9EA4-A9988B5ABC38}" name="Resource Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7656305F-8A5C-47DD-B30F-A5A2DDF6BA3B}" name="In-progress" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{01F03680-387B-4396-881D-D8692076CAFB}" name="Done" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C8B16ACA-3649-43AE-9870-DA150B8F4C27}" name="Discarded / Hold" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{94E9160D-5E84-446E-9333-D6366B7E94A9}" name="Hours Spent - Project" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{71FCC1BB-CD17-411D-84B5-72A33C3D732E}" name="Hours Spent - Non Project" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{AD223263-251D-4364-922D-657CA0BF6FED}" name="Comments" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{396EF6F7-EC64-4D4E-8E01-69FB9BDB9A54}" name="Table375111719212325" displayName="Table375111719212325" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="B2:E4" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{84A3FC7B-02E6-44DB-98AA-6783349E3D38}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4C90FA59-2548-4B68-BBFB-E6DE9B9B243A}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{23DB2E45-3FE0-4350-8C54-7D8B45F36289}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4AC2DE38-C7EC-48C4-93E9-CB48E45B0F9C}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowBorderDxfId="206" tableBorderDxfId="207" totalsRowBorderDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="230" dataDxfId="229" headerRowBorderDxfId="227" tableBorderDxfId="228" totalsRowBorderDxfId="226">
   <autoFilter ref="B8:H18" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="204"/>
-    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="203"/>
-    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="202"/>
-    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="201"/>
-    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="200"/>
-    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="199"/>
-    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="198"/>
+    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="225"/>
+    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="224"/>
+    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="223"/>
+    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="222"/>
+    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="221"/>
+    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="220"/>
+    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="219"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196" headerRowBorderDxfId="194" tableBorderDxfId="195" totalsRowBorderDxfId="193">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217" headerRowBorderDxfId="215" tableBorderDxfId="216" totalsRowBorderDxfId="214">
   <autoFilter ref="B3:E5" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="192"/>
-    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="191"/>
-    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="190"/>
-    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="189"/>
+    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="213"/>
+    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="212"/>
+    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="211"/>
+    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="210"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowBorderDxfId="206" tableBorderDxfId="207" totalsRowBorderDxfId="205">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="182"/>
-    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="181"/>
-    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="180"/>
-    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="179"/>
-    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="178"/>
-    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="203"/>
+    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="202"/>
+    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="201"/>
+    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="200"/>
+    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="199"/>
+    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196" headerRowBorderDxfId="194" tableBorderDxfId="195" totalsRowBorderDxfId="193">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="171"/>
-    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="170"/>
-    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="169"/>
-    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="168"/>
+    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="191"/>
+    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="190"/>
+    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="177"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="168"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8350,8 +8920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F129C-4B66-4886-90DA-03408C042996}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8614,6 +9184,323 @@
       </c>
       <c r="H15" s="26"/>
     </row>
+    <row r="16" spans="1:8" ht="284.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" ht="273.75" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="42">
+        <v>3</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FFC9C9-2848-4E62-84AF-44A9BCE5AD3F}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="21">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="21">
+      <c r="B4" s="6"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="41.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="219.75" customHeight="1">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="185.25" customHeight="1">
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="G9" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="147" customHeight="1">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="229.5" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" ht="186.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="192" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>3.2</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="196.5" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="45">
+        <v>3.2</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
     <row r="16" spans="1:8" ht="197.25" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>34</v>
@@ -8622,7 +9509,7 @@
         <v>191</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35">

</xml_diff>

<commit_message>
Updated Timesheet - Prithvi
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet .xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE2E045-D169-4233-9266-E1442909352D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{641B0531-80D7-4B53-A63A-E3D5C196BC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="216">
   <si>
     <t>Column1</t>
   </si>
@@ -849,10 +849,10 @@
                                                   </t>
   </si>
   <si>
-    <t xml:space="preserve">8.45 to 9.00 am (15mins): Brainstorming with team 
+    <t>8.45 to 9.00 am (15mins): Brainstorming with team 
 9.10 to 10.30 am (1hr 20mins) : Refined Drive entity, Location Entity , Response Entity Operations
 11.00 to 12.00 (1hr): Refined Employee Operations 
-</t>
+12.00 : absent</t>
   </si>
   <si>
     <t>8:45 to 9:00  - Brainstorming
@@ -884,6 +884,15 @@
 10.45 am - 11.15 am : Google API - calender (Event,calender list, settings) and Google workspace.
 11:15 am - 12:15 pm : converting sheets to document format. (NFR)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      Have to work on Api Implementations</t>
+  </si>
+  <si>
+    <t>9:30am to 10:00am : Brainstorming with team    
+10.10am to 11.30 am : Implemented Role Service and Role Model for API
+12.00pm to 12.30pm : Worked on EF Code First for Role Model class 
+12.30pm to 1.00 : System Allocation.</t>
   </si>
   <si>
     <t xml:space="preserve"> 9:30 to 10:00 -Brainstorming with team                             10:00 to 10:30 - Working on layout for TAC's Upcoming drive.                                                                                          10:30 to 11:30 - Session with rafi.                                        11:30 to 11:45 - Break                                                           11:45 to 12:30 - continued on desiging the upcoming drives page .</t>
@@ -9884,323 +9893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C80E3FE-E1B7-4355-8FC5-626F5977EF65}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-    <col min="5" max="5" width="62.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="21">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="21">
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="21">
-      <c r="B4" s="6"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="21">
-      <c r="B5" s="4"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="20.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="41.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="219.75" customHeight="1">
-      <c r="B8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="35">
-        <v>1</v>
-      </c>
-      <c r="G8" s="35">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8" ht="185.25" customHeight="1">
-      <c r="B9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="35">
-        <v>3</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="H9" s="24"/>
-    </row>
-    <row r="10" spans="1:8" ht="147" customHeight="1">
-      <c r="B10" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="35">
-        <v>3</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:8" ht="229.5" customHeight="1">
-      <c r="B11" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="35">
-        <v>4</v>
-      </c>
-      <c r="G11" s="35">
-        <v>0</v>
-      </c>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:8" ht="186.75" customHeight="1">
-      <c r="B12" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1">
-      <c r="B13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="G13" s="35">
-        <v>0</v>
-      </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1">
-      <c r="B14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="35">
-        <v>3.5</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1">
-      <c r="B15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="45">
-        <v>3</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1">
-      <c r="B16" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35">
-        <v>3.5</v>
-      </c>
-      <c r="G16" s="35">
-        <v>0</v>
-      </c>
-      <c r="H16" s="27"/>
-    </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1">
-      <c r="B17" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="42">
-        <v>2.5</v>
-      </c>
-      <c r="G17" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="H17" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FFC9C9-2848-4E62-84AF-44A9BCE5AD3F}">
-  <dimension ref="A2:H17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10429,7 +10123,7 @@
         <v>167</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
@@ -10447,7 +10141,324 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="45">
+        <v>3</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" ht="273.75" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FFC9C9-2848-4E62-84AF-44A9BCE5AD3F}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="21">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="21">
+      <c r="B4" s="6"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="41.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="219.75" customHeight="1">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="185.25" customHeight="1">
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35">
+        <v>3</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="147" customHeight="1">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>3</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="229.5" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" ht="186.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="192" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="44" t="s">
         <v>213</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="196.5" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>215</v>
       </c>
       <c r="D15" s="47" t="s">
         <v>207</v>

</xml_diff>